<commit_message>
Added Powerball odds to master data sheet.
</commit_message>
<xml_diff>
--- a/data/master.xlsx
+++ b/data/master.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bearc\Desktop\Code\voting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245B8C9C-CB41-491C-B12A-8A92E725A7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768F2902-8113-469B-8795-DECA73BF4E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4416" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00912FA7-5E26-4F82-8A5B-1284969E2121}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00912FA7-5E26-4F82-8A5B-1284969E2121}"/>
   </bookViews>
   <sheets>
     <sheet name="State Pop 18+" sheetId="3" r:id="rId1"/>
+    <sheet name="Powerball" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="SCPRC_18_POP_RES_REG">#REF!</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>State</t>
   </si>
@@ -187,13 +188,80 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Odds of Winning</t>
+  </si>
+  <si>
+    <t>Prize</t>
+  </si>
+  <si>
+    <t>5 plus Powerball</t>
+  </si>
+  <si>
+    <t>1 in 292,201,338</t>
+  </si>
+  <si>
+    <t>Jackpot</t>
+  </si>
+  <si>
+    <t>1 in 11,688,054</t>
+  </si>
+  <si>
+    <t>$1 million</t>
+  </si>
+  <si>
+    <t>4 plus Powerball</t>
+  </si>
+  <si>
+    <t>1 in 913,130</t>
+  </si>
+  <si>
+    <t>1 in 36,525</t>
+  </si>
+  <si>
+    <t>3 plus Powerball</t>
+  </si>
+  <si>
+    <t>1 in 14,494</t>
+  </si>
+  <si>
+    <t>1 in 580</t>
+  </si>
+  <si>
+    <t>2 plus Powerball</t>
+  </si>
+  <si>
+    <t>1 in 701</t>
+  </si>
+  <si>
+    <t>1 plus Powerball</t>
+  </si>
+  <si>
+    <t>1 in 92</t>
+  </si>
+  <si>
+    <t>Powerball</t>
+  </si>
+  <si>
+    <t>1 in 38</t>
+  </si>
+  <si>
+    <t>Odds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +277,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -234,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -243,6 +326,18 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D7935D-8C65-46C0-B4A9-A7F7FA27BEA9}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -990,4 +1085,175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F83810-D696-46A3-BF16-129103E7DD4F}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <f>1/292201338</f>
+        <v>3.4222978130237033E-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <f>1/11688054</f>
+        <v>8.555744181195603E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D4">
+        <f>1/913130</f>
+        <v>1.0951343182241301E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="7">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <f>1/36525</f>
+        <v>2.7378507871321012E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="7">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <f>1/14494</f>
+        <v>6.8994066510280109E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f>1/580</f>
+        <v>1.7241379310344827E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f>1/701</f>
+        <v>1.4265335235378032E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f>1/92</f>
+        <v>1.0869565217391304E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>